<commit_message>
Test support for hyperlinks
</commit_message>
<xml_diff>
--- a/test/fixtures/test.xlsx
+++ b/test/fixtures/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -68,6 +68,20 @@
   <si>
     <t>not ticked</t>
   </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://elixir-lang.org/</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -81,7 +95,7 @@
     <numFmt numFmtId="62" formatCode="0.0%"/>
     <numFmt numFmtId="63" formatCode="[$CHF]&quot; &quot;0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -101,6 +115,12 @@
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="14"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -347,6 +367,7 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2156,13 +2177,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="17" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="17" customWidth="1"/>
+    <col min="2" max="2" width="22.7734" style="17" customWidth="1"/>
     <col min="3" max="256" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2185,7 +2207,7 @@
       </c>
       <c r="B3" s="20">
         <f>NOW()</f>
-        <v>43787.924259259256</v>
+        <v>43793.462650462963</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
@@ -2237,7 +2259,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s" s="24">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" location="" tooltip="" display="https://elixir-lang.org/"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Add support for additional custom formats
</commit_message>
<xml_diff>
--- a/test/fixtures/test.xlsx
+++ b/test/fixtures/test.xlsx
@@ -93,7 +93,7 @@
     <numFmt numFmtId="60" formatCode="dd/mm/yyyy hh:mm"/>
     <numFmt numFmtId="61" formatCode="hh:mm"/>
     <numFmt numFmtId="62" formatCode="0.0%"/>
-    <numFmt numFmtId="63" formatCode="[$CHF]&quot; &quot;0.00"/>
+    <numFmt numFmtId="63" formatCode="[$CHF]0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1436,7 +1436,7 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2086,7 +2086,7 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="5" width="16.3516" style="9" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2184,8 +2184,8 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="17" customWidth="1"/>
-    <col min="2" max="2" width="22.7734" style="17" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="17" customWidth="1"/>
+    <col min="2" max="2" width="22.8516" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="B3" s="20">
         <f>NOW()</f>
-        <v>43793.462650462963</v>
+        <v>43990.893761574072</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">

</xml_diff>